<commit_message>
Adjust number format in test data
</commit_message>
<xml_diff>
--- a/Test 1 Data.xlsx
+++ b/Test 1 Data.xlsx
@@ -84,9 +84,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="hh:mm:ss.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -120,12 +121,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -422,9 +423,9 @@
     <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -453,13 +454,13 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
@@ -467,7 +468,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
@@ -491,14 +492,14 @@
       <c r="H2" s="1">
         <v>63</v>
       </c>
-      <c r="I2" s="5">
-        <f>G2/H2</f>
+      <c r="I2" s="4">
+        <f t="shared" ref="I2:I33" si="0">G2/H2</f>
         <v>23.031746031746032</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>1.9675925932993721E-7</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="5">
         <v>0.26984126993819962</v>
       </c>
       <c r="L2" t="s">
@@ -506,7 +507,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -530,14 +531,14 @@
       <c r="H3" s="1">
         <v>432</v>
       </c>
-      <c r="I3" s="5">
-        <f>G3/H3</f>
+      <c r="I3" s="4">
+        <f t="shared" si="0"/>
         <v>35.75</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="5">
         <v>2.3148148287077674E-3</v>
       </c>
       <c r="L3" t="s">
@@ -545,7 +546,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4">
@@ -569,14 +570,14 @@
       <c r="H4" s="1">
         <v>1728</v>
       </c>
-      <c r="I4" s="5">
-        <f>G4/H4</f>
+      <c r="I4" s="4">
+        <f t="shared" si="0"/>
         <v>47.93113425925926</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="5">
         <v>0</v>
       </c>
       <c r="L4" t="s">
@@ -584,7 +585,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5">
@@ -608,14 +609,14 @@
       <c r="H5" s="1">
         <v>3969</v>
       </c>
-      <c r="I5" s="5">
-        <f>G5/H5</f>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
         <v>56.96724615772235</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="5">
         <v>2.5195263441717196E-4</v>
       </c>
       <c r="L5" t="s">
@@ -623,7 +624,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6">
@@ -647,14 +648,14 @@
       <c r="H6" s="1">
         <v>10449</v>
       </c>
-      <c r="I6" s="5">
-        <f>G6/H6</f>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
         <v>66.590295722078665</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>1.1574073921494232E-8</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="5">
         <v>9.570293681855696E-5</v>
       </c>
       <c r="L6" t="s">
@@ -662,7 +663,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7">
@@ -686,14 +687,14 @@
       <c r="H7" s="1">
         <v>56382</v>
       </c>
-      <c r="I7" s="5">
-        <f>G7/H7</f>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
         <v>78.111915150225244</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>5.7870370384627279E-8</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="5">
         <v>8.8680784669429907E-5</v>
       </c>
       <c r="L7" t="s">
@@ -701,7 +702,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8">
@@ -725,14 +726,14 @@
       <c r="H8" s="1">
         <v>1077561</v>
       </c>
-      <c r="I8" s="5">
-        <f>G8/H8</f>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
         <v>87.930854030537489</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>1.1342592592944456E-6</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="5">
         <v>9.0946127414633701E-5</v>
       </c>
       <c r="L8" t="s">
@@ -740,7 +741,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9">
@@ -764,14 +765,14 @@
       <c r="H9" s="1">
         <v>214494</v>
       </c>
-      <c r="I9" s="5">
-        <f>G9/H9</f>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
         <v>100.70313854933005</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>2.4305555568204795E-7</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="5">
         <v>9.790483654987526E-5</v>
       </c>
       <c r="L9" t="s">
@@ -779,7 +780,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10">
@@ -803,14 +804,14 @@
       <c r="H10" s="1">
         <v>3464271</v>
       </c>
-      <c r="I10" s="5">
-        <f>G10/H10</f>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
         <v>108.35157382317954</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>4.5254629630342436E-6</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="5">
         <v>1.1286645877477791E-4</v>
       </c>
       <c r="L10" t="s">
@@ -818,7 +819,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11">
@@ -842,14 +843,14 @@
       <c r="H11" s="1">
         <v>36003</v>
       </c>
-      <c r="I11" s="5">
-        <f>G11/H11</f>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
         <v>121.41252117879066</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>5.7870370273604976E-8</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="5">
         <v>1.3887731554702303E-4</v>
       </c>
       <c r="L11" t="s">
@@ -857,7 +858,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12">
@@ -881,14 +882,14 @@
       <c r="H12" s="1">
         <v>21</v>
       </c>
-      <c r="I12" s="5">
-        <f>G12/H12</f>
+      <c r="I12" s="4">
+        <f t="shared" si="0"/>
         <v>154.9047619047619</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="5">
         <v>4.7619047904845502E-2</v>
       </c>
       <c r="L12" t="s">
@@ -896,7 +897,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13">
@@ -920,14 +921,14 @@
       <c r="H13" s="1">
         <v>60</v>
       </c>
-      <c r="I13" s="5">
-        <f>G13/H13</f>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
         <v>261.55</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <v>1.1574074032516535E-8</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="5">
         <v>1.666666660682381E-2</v>
       </c>
       <c r="L13" t="s">
@@ -935,7 +936,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14">
@@ -959,14 +960,14 @@
       <c r="H14" s="1">
         <v>216</v>
       </c>
-      <c r="I14" s="5">
-        <f>G14/H14</f>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
         <v>302.95833333333331</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="3">
         <v>2.3148148176055372E-8</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="5">
         <v>9.2592592704221488E-3</v>
       </c>
       <c r="L14" t="s">
@@ -974,7 +975,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -998,14 +999,14 @@
       <c r="H15" s="1">
         <v>51</v>
       </c>
-      <c r="I15" s="5">
-        <f>G15/H15</f>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
         <v>394.39215686274508</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <v>0</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="5">
         <v>0</v>
       </c>
       <c r="L15" t="s">
@@ -1013,7 +1014,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -1037,14 +1038,14 @@
       <c r="H16" s="1">
         <v>495</v>
       </c>
-      <c r="I16" s="5">
-        <f>G16/H16</f>
+      <c r="I16" s="4">
+        <f t="shared" si="0"/>
         <v>322.69494949494947</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="5">
         <v>2.0202020323267789E-3</v>
       </c>
       <c r="L16" t="s">
@@ -1052,7 +1053,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B17">
@@ -1076,14 +1077,14 @@
       <c r="H17" s="1">
         <v>972</v>
       </c>
-      <c r="I17" s="5">
-        <f>G17/H17</f>
+      <c r="I17" s="4">
+        <f t="shared" si="0"/>
         <v>383.14711934156378</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="5">
         <v>1.0288065905367854E-3</v>
       </c>
       <c r="L17" t="s">
@@ -1091,7 +1092,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B18">
@@ -1115,14 +1116,14 @@
       <c r="H18" s="1">
         <v>6195</v>
       </c>
-      <c r="I18" s="5">
-        <f>G18/H18</f>
+      <c r="I18" s="4">
+        <f t="shared" si="0"/>
         <v>370.47974172719938</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="3">
         <v>1.0416666673673802E-7</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="5">
         <v>1.4527845046092276E-3</v>
       </c>
       <c r="L18" t="s">
@@ -1130,7 +1131,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -1154,14 +1155,14 @@
       <c r="H19" s="1">
         <v>606</v>
       </c>
-      <c r="I19" s="5">
-        <f>G19/H19</f>
+      <c r="I19" s="4">
+        <f t="shared" si="0"/>
         <v>436.93069306930693</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="3">
         <v>0</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="5">
         <v>0</v>
       </c>
       <c r="L19" t="s">
@@ -1169,7 +1170,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B20">
@@ -1193,14 +1194,14 @@
       <c r="H20" s="1">
         <v>1605</v>
       </c>
-      <c r="I20" s="5">
-        <f>G20/H20</f>
+      <c r="I20" s="4">
+        <f t="shared" si="0"/>
         <v>456.77694704049844</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="3">
         <v>2.3148148176055372E-8</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="5">
         <v>1.2461059205054108E-3</v>
       </c>
       <c r="L20" t="s">
@@ -1208,7 +1209,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B21">
@@ -1232,14 +1233,14 @@
       <c r="H21" s="1">
         <v>723</v>
       </c>
-      <c r="I21" s="5">
-        <f>G21/H21</f>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
         <v>538.64453665283543</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="5">
         <v>1.3831258727548487E-3</v>
       </c>
       <c r="L21" t="s">
@@ -1247,7 +1248,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B22">
@@ -1271,14 +1272,14 @@
       <c r="H22" s="1">
         <v>15</v>
       </c>
-      <c r="I22" s="5">
-        <f>G22/H22</f>
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
         <v>913.66666666666663</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="3">
         <v>2.314814806503307E-8</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="5">
         <v>0.13333333285459048</v>
       </c>
       <c r="L22" t="s">
@@ -1286,7 +1287,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B23">
@@ -1310,14 +1311,14 @@
       <c r="H23" s="1">
         <v>6</v>
       </c>
-      <c r="I23" s="5">
-        <f>G23/H23</f>
+      <c r="I23" s="4">
+        <f t="shared" si="0"/>
         <v>6307.166666666667</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="5">
         <v>0.16666666766695926</v>
       </c>
       <c r="L23" t="s">
@@ -1325,7 +1326,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B24">
@@ -1349,14 +1350,14 @@
       <c r="H24" s="1">
         <v>48</v>
       </c>
-      <c r="I24" s="5">
-        <f>G24/H24</f>
+      <c r="I24" s="4">
+        <f t="shared" si="0"/>
         <v>8770.8958333333339</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="3">
         <v>9.2592592593199186E-8</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="5">
         <v>0.16666666666775853</v>
       </c>
       <c r="L24" t="s">
@@ -1364,7 +1365,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B25">
@@ -1388,14 +1389,14 @@
       <c r="H25" s="1">
         <v>21</v>
       </c>
-      <c r="I25" s="5">
-        <f>G25/H25</f>
+      <c r="I25" s="4">
+        <f t="shared" si="0"/>
         <v>15718.619047619048</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="3">
         <v>3.4722222208571907E-8</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="5">
         <v>0.14285714280098155</v>
       </c>
       <c r="L25" t="s">
@@ -1403,7 +1404,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B26">
@@ -1427,14 +1428,14 @@
       <c r="H26" s="1">
         <v>45</v>
       </c>
-      <c r="I26" s="5">
-        <f>G26/H26</f>
+      <c r="I26" s="4">
+        <f t="shared" si="0"/>
         <v>15563.622222222222</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="3">
         <v>6.9444444417143814E-8</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="5">
         <v>0.13333333328091612</v>
       </c>
       <c r="L26" t="s">
@@ -1442,7 +1443,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B27">
@@ -1466,14 +1467,14 @@
       <c r="H27" s="1">
         <v>6</v>
       </c>
-      <c r="I27" s="5">
-        <f>G27/H27</f>
+      <c r="I27" s="4">
+        <f t="shared" si="0"/>
         <v>34068.666666666664</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="3">
         <v>2.3148148176055372E-8</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="5">
         <v>0.33333333373519736</v>
       </c>
       <c r="L27" t="s">
@@ -1481,7 +1482,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B28">
@@ -1505,14 +1506,14 @@
       <c r="H28" s="1">
         <v>123</v>
       </c>
-      <c r="I28" s="5">
-        <f>G28/H28</f>
+      <c r="I28" s="4">
+        <f t="shared" si="0"/>
         <v>25625.422764227642</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="3">
         <v>1.620370371213653E-7</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="5">
         <v>0.11382113827061757</v>
       </c>
       <c r="L28" t="s">
@@ -1520,7 +1521,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B29">
@@ -1544,14 +1545,14 @@
       <c r="H29" s="1">
         <v>120</v>
       </c>
-      <c r="I29" s="5">
-        <f>G29/H29</f>
+      <c r="I29" s="4">
+        <f t="shared" si="0"/>
         <v>24300.708333333332</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="3">
         <v>1.3888888883428763E-7</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="5">
         <v>9.9999999960687092E-2</v>
       </c>
       <c r="L29" t="s">
@@ -1559,7 +1560,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30">
@@ -1583,14 +1584,14 @@
       <c r="H30" s="1">
         <v>39</v>
       </c>
-      <c r="I30" s="5">
-        <f>G30/H30</f>
+      <c r="I30" s="4">
+        <f t="shared" si="0"/>
         <v>49433.179487179485</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30" s="3">
         <v>1.0416666651469342E-7</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="5">
         <v>0.23076923043255157</v>
       </c>
       <c r="L30" t="s">
@@ -1598,7 +1599,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B31">
@@ -1622,14 +1623,14 @@
       <c r="H31" s="1">
         <v>39</v>
       </c>
-      <c r="I31" s="5">
-        <f>G31/H31</f>
+      <c r="I31" s="4">
+        <f t="shared" si="0"/>
         <v>36829.564102564102</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="3">
         <v>6.9444444417143814E-8</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="5">
         <v>0.15384615378567246</v>
       </c>
       <c r="L31" t="s">
@@ -1637,7 +1638,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B32">
@@ -1661,14 +1662,14 @@
       <c r="H32" s="1">
         <v>100000000</v>
       </c>
-      <c r="I32" s="5">
-        <f>G32/H32</f>
+      <c r="I32" s="4">
+        <f t="shared" si="0"/>
         <v>2487.0000020000002</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="3">
         <v>7.0861111111120145E-3</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="5">
         <v>6.1224000000007798E-3</v>
       </c>
       <c r="L32" t="s">
@@ -1676,7 +1677,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B33">
@@ -1700,14 +1701,14 @@
       <c r="H33" s="1">
         <v>100000000</v>
       </c>
-      <c r="I33" s="5">
-        <f>G33/H33</f>
+      <c r="I33" s="4">
+        <f t="shared" si="0"/>
         <v>5645.0000019999998</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="3">
         <v>1.3430092592591203E-2</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="5">
         <v>1.1603599999998798E-2</v>
       </c>
       <c r="L33" t="s">
@@ -1715,7 +1716,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B34">
@@ -1739,14 +1740,14 @@
       <c r="H34" s="1">
         <v>100000000</v>
       </c>
-      <c r="I34" s="5">
-        <f>G34/H34</f>
+      <c r="I34" s="4">
+        <f t="shared" ref="I34:I65" si="1">G34/H34</f>
         <v>8895.0000020000007</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="3">
         <v>2.1347222222221074E-2</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="5">
         <v>1.844399999999901E-2</v>
       </c>
       <c r="L34" t="s">
@@ -1754,7 +1755,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B35">
@@ -1778,14 +1779,14 @@
       <c r="H35" s="1">
         <v>100000000</v>
       </c>
-      <c r="I35" s="5">
-        <f>G35/H35</f>
+      <c r="I35" s="4">
+        <f t="shared" si="1"/>
         <v>11593.000002000001</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="3">
         <v>2.6320254629630391E-2</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="5">
         <v>2.2740700000000658E-2</v>
       </c>
       <c r="L35" t="s">
@@ -1793,7 +1794,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B36">
@@ -1817,14 +1818,14 @@
       <c r="H36" s="1">
         <v>100000000</v>
       </c>
-      <c r="I36" s="5">
-        <f>G36/H36</f>
+      <c r="I36" s="4">
+        <f t="shared" si="1"/>
         <v>15395.000002000001</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="3">
         <v>3.2776157407408135E-2</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="5">
         <v>2.8318600000000627E-2</v>
       </c>
       <c r="L36" t="s">
@@ -1832,7 +1833,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B37">
@@ -1856,14 +1857,14 @@
       <c r="H37" s="1">
         <v>100000000</v>
       </c>
-      <c r="I37" s="5">
-        <f>G37/H37</f>
+      <c r="I37" s="4">
+        <f t="shared" si="1"/>
         <v>18369.000002000001</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="3">
         <v>3.9829166666665028E-2</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="5">
         <v>3.4412399999998587E-2</v>
       </c>
       <c r="L37" t="s">
@@ -1871,7 +1872,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B38">
@@ -1895,14 +1896,14 @@
       <c r="H38" s="1">
         <v>100000000</v>
       </c>
-      <c r="I38" s="5">
-        <f>G38/H38</f>
+      <c r="I38" s="4">
+        <f t="shared" si="1"/>
         <v>21527.000002000001</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="3">
         <v>4.6798032407405765E-2</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="5">
         <v>4.0433499999998575E-2</v>
       </c>
       <c r="L38" t="s">
@@ -1910,7 +1911,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B39">
@@ -1934,14 +1935,14 @@
       <c r="H39" s="1">
         <v>100000000</v>
       </c>
-      <c r="I39" s="5">
-        <f>G39/H39</f>
+      <c r="I39" s="4">
+        <f t="shared" si="1"/>
         <v>24685.000002000001</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="3">
         <v>5.2787847222223183E-2</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="5">
         <v>4.5608700000000842E-2</v>
       </c>
       <c r="L39" t="s">
@@ -1949,7 +1950,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B40">
@@ -1973,14 +1974,14 @@
       <c r="H40" s="1">
         <v>100000000</v>
       </c>
-      <c r="I40" s="5">
-        <f>G40/H40</f>
+      <c r="I40" s="4">
+        <f t="shared" si="1"/>
         <v>27935.000002000001</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="3">
         <v>7.4834953703705187E-2</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="5">
         <v>6.4657400000001281E-2</v>
       </c>
       <c r="L40" t="s">
@@ -1988,7 +1989,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B41">
@@ -2012,14 +2013,14 @@
       <c r="H41" s="1">
         <v>100000000</v>
       </c>
-      <c r="I41" s="5">
-        <f>G41/H41</f>
+      <c r="I41" s="4">
+        <f t="shared" si="1"/>
         <v>30725.000002000001</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="3">
         <v>6.4717708333332791E-2</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="5">
         <v>5.5916099999999531E-2</v>
       </c>
       <c r="L41" t="s">
@@ -2027,7 +2028,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B42">
@@ -2051,14 +2052,14 @@
       <c r="H42" s="1">
         <v>10</v>
       </c>
-      <c r="I42" s="5">
-        <f>G42/H42</f>
+      <c r="I42" s="4">
+        <f t="shared" si="1"/>
         <v>22.1</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="3">
         <v>0</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="5">
         <v>0</v>
       </c>
       <c r="L42" t="s">
@@ -2066,7 +2067,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B43">
@@ -2090,14 +2091,14 @@
       <c r="H43" s="1">
         <v>131</v>
       </c>
-      <c r="I43" s="5">
-        <f>G43/H43</f>
+      <c r="I43" s="4">
+        <f t="shared" si="1"/>
         <v>35.885496183206108</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="5">
         <v>7.6335878320744699E-3</v>
       </c>
       <c r="L43" t="s">
@@ -2105,7 +2106,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B44">
@@ -2129,14 +2130,14 @@
       <c r="H44" s="1">
         <v>1526</v>
       </c>
-      <c r="I44" s="5">
-        <f>G44/H44</f>
+      <c r="I44" s="4">
+        <f t="shared" si="1"/>
         <v>48.473787680209696</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="3">
         <v>0</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="5">
         <v>0</v>
       </c>
       <c r="L44" t="s">
@@ -2144,7 +2145,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B45">
@@ -2168,14 +2169,14 @@
       <c r="H45" s="1">
         <v>126320</v>
       </c>
-      <c r="I45" s="5">
-        <f>G45/H45</f>
+      <c r="I45" s="4">
+        <f t="shared" si="1"/>
         <v>56.879924002533251</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45" s="3">
         <v>1.2731481480177109E-7</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="5">
         <v>8.708043064338998E-5</v>
       </c>
       <c r="L45" t="s">
@@ -2183,7 +2184,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B46">
@@ -2207,14 +2208,14 @@
       <c r="H46" s="1">
         <v>50</v>
       </c>
-      <c r="I46" s="5">
-        <f>G46/H46</f>
+      <c r="I46" s="4">
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="J46" s="4">
+      <c r="J46" s="3">
         <v>0</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="5">
         <v>0</v>
       </c>
       <c r="L46" t="s">
@@ -2222,7 +2223,7 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B47">
@@ -2246,14 +2247,14 @@
       <c r="H47" s="1">
         <v>6147</v>
       </c>
-      <c r="I47" s="5">
-        <f>G47/H47</f>
+      <c r="I47" s="4">
+        <f t="shared" si="1"/>
         <v>76.935903692858304</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J47" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="5">
         <v>1.6268098356950634E-4</v>
       </c>
       <c r="L47" t="s">
@@ -2261,7 +2262,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B48">
@@ -2285,14 +2286,14 @@
       <c r="H48" s="1">
         <v>10618</v>
       </c>
-      <c r="I48" s="5">
-        <f>G48/H48</f>
+      <c r="I48" s="4">
+        <f t="shared" si="1"/>
         <v>87.896213976266722</v>
       </c>
-      <c r="J48" s="4">
+      <c r="J48" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="5">
         <v>9.4179695423032169E-5</v>
       </c>
       <c r="L48" t="s">
@@ -2300,7 +2301,7 @@
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B49">
@@ -2324,14 +2325,14 @@
       <c r="H49" s="1">
         <v>446075</v>
       </c>
-      <c r="I49" s="5">
-        <f>G49/H49</f>
+      <c r="I49" s="4">
+        <f t="shared" si="1"/>
         <v>101.69146219806086</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J49" s="3">
         <v>4.86111111031029E-7</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K49" s="5">
         <v>9.4154570404261402E-5</v>
       </c>
       <c r="L49" t="s">
@@ -2339,7 +2340,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B50">
@@ -2363,14 +2364,14 @@
       <c r="H50" s="1">
         <v>175668413</v>
       </c>
-      <c r="I50" s="5">
-        <f>G50/H50</f>
+      <c r="I50" s="4">
+        <f t="shared" si="1"/>
         <v>108.20989820748252</v>
       </c>
-      <c r="J50" s="4">
+      <c r="J50" s="3">
         <v>1.9484953703696739E-4</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K50" s="5">
         <v>9.5833961908644224E-5</v>
       </c>
       <c r="L50" t="s">
@@ -2378,7 +2379,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B51">
@@ -2402,14 +2403,14 @@
       <c r="H51" s="1">
         <v>260286064213</v>
       </c>
-      <c r="I51" s="5">
-        <f>G51/H51</f>
+      <c r="I51" s="4">
+        <f t="shared" si="1"/>
         <v>118.50206108108831</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51" s="3">
         <v>0.26727133101851852</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K51" s="5">
         <v>8.8718706742220817E-5</v>
       </c>
       <c r="L51" t="s">
@@ -2417,7 +2418,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B52">
@@ -2441,14 +2442,14 @@
       <c r="H52" s="1">
         <v>10</v>
       </c>
-      <c r="I52" s="5">
-        <f>G52/H52</f>
+      <c r="I52" s="4">
+        <f t="shared" si="1"/>
         <v>74.8</v>
       </c>
-      <c r="J52" s="4">
+      <c r="J52" s="3">
         <v>1.1574074032516535E-8</v>
       </c>
-      <c r="K52" s="2">
+      <c r="K52" s="5">
         <v>9.999999964094286E-2</v>
       </c>
       <c r="L52" t="s">
@@ -2456,7 +2457,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B53">
@@ -2480,14 +2481,14 @@
       <c r="H53" s="1">
         <v>63</v>
       </c>
-      <c r="I53" s="5">
-        <f>G53/H53</f>
+      <c r="I53" s="4">
+        <f t="shared" si="1"/>
         <v>86.365079365079367</v>
       </c>
-      <c r="J53" s="4">
+      <c r="J53" s="3">
         <v>0</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K53" s="5">
         <v>0</v>
       </c>
       <c r="L53" t="s">
@@ -2495,7 +2496,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B54">
@@ -2519,14 +2520,14 @@
       <c r="H54" s="1">
         <v>241</v>
       </c>
-      <c r="I54" s="5">
-        <f>G54/H54</f>
+      <c r="I54" s="4">
+        <f t="shared" si="1"/>
         <v>123.96265560165975</v>
       </c>
-      <c r="J54" s="4">
+      <c r="J54" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K54" s="2">
+      <c r="K54" s="5">
         <v>4.1493776182645456E-3</v>
       </c>
       <c r="L54" t="s">
@@ -2534,7 +2535,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B55">
@@ -2558,14 +2559,14 @@
       <c r="H55" s="1">
         <v>349</v>
       </c>
-      <c r="I55" s="5">
-        <f>G55/H55</f>
+      <c r="I55" s="4">
+        <f t="shared" si="1"/>
         <v>181.91977077363896</v>
       </c>
-      <c r="J55" s="4">
+      <c r="J55" s="3">
         <v>0</v>
       </c>
-      <c r="K55" s="2">
+      <c r="K55" s="5">
         <v>0</v>
       </c>
       <c r="L55" t="s">
@@ -2573,7 +2574,7 @@
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B56">
@@ -2597,14 +2598,14 @@
       <c r="H56" s="1">
         <v>50</v>
       </c>
-      <c r="I56" s="5">
-        <f>G56/H56</f>
+      <c r="I56" s="4">
+        <f t="shared" si="1"/>
         <v>144.62</v>
       </c>
-      <c r="J56" s="4">
+      <c r="J56" s="3">
         <v>1.1574074032516535E-8</v>
       </c>
-      <c r="K56" s="2">
+      <c r="K56" s="5">
         <v>1.9999999928188572E-2</v>
       </c>
       <c r="L56" t="s">
@@ -2612,7 +2613,7 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B57">
@@ -2636,14 +2637,14 @@
       <c r="H57" s="1">
         <v>65</v>
       </c>
-      <c r="I57" s="5">
-        <f>G57/H57</f>
+      <c r="I57" s="4">
+        <f t="shared" si="1"/>
         <v>153.2923076923077</v>
       </c>
-      <c r="J57" s="4">
+      <c r="J57" s="3">
         <v>0</v>
       </c>
-      <c r="K57" s="2">
+      <c r="K57" s="5">
         <v>0</v>
       </c>
       <c r="L57" t="s">
@@ -2651,7 +2652,7 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B58">
@@ -2675,14 +2676,14 @@
       <c r="H58" s="1">
         <v>332</v>
       </c>
-      <c r="I58" s="5">
-        <f>G58/H58</f>
+      <c r="I58" s="4">
+        <f t="shared" si="1"/>
         <v>187.85240963855421</v>
       </c>
-      <c r="J58" s="4">
+      <c r="J58" s="3">
         <v>0</v>
       </c>
-      <c r="K58" s="2">
+      <c r="K58" s="5">
         <v>0</v>
       </c>
       <c r="L58" t="s">
@@ -2690,7 +2691,7 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B59">
@@ -2714,14 +2715,14 @@
       <c r="H59" s="1">
         <v>3395</v>
       </c>
-      <c r="I59" s="5">
-        <f>G59/H59</f>
+      <c r="I59" s="4">
+        <f t="shared" si="1"/>
         <v>196.95051546391753</v>
       </c>
-      <c r="J59" s="4">
+      <c r="J59" s="3">
         <v>1.1574074032516535E-8</v>
       </c>
-      <c r="K59" s="2">
+      <c r="K59" s="5">
         <v>2.9455080895712181E-4</v>
       </c>
       <c r="L59" t="s">
@@ -2729,7 +2730,7 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B60">
@@ -2753,14 +2754,14 @@
       <c r="H60" s="1">
         <v>235764</v>
       </c>
-      <c r="I60" s="5">
-        <f>G60/H60</f>
+      <c r="I60" s="4">
+        <f t="shared" si="1"/>
         <v>203.71493103272763</v>
       </c>
-      <c r="J60" s="4">
+      <c r="J60" s="3">
         <v>1.3541666666894159E-6</v>
       </c>
-      <c r="K60" s="2">
+      <c r="K60" s="5">
         <v>4.9625897084357889E-4</v>
       </c>
       <c r="L60" t="s">
@@ -2768,7 +2769,7 @@
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B61">
@@ -2792,14 +2793,14 @@
       <c r="H61" s="1">
         <v>2183291698</v>
       </c>
-      <c r="I61" s="5">
-        <f>G61/H61</f>
+      <c r="I61" s="4">
+        <f t="shared" si="1"/>
         <v>193.90434788205749</v>
       </c>
-      <c r="J61" s="4">
+      <c r="J61" s="3">
         <v>9.6898611111110866E-3</v>
       </c>
-      <c r="K61" s="2">
+      <c r="K61" s="5">
         <v>3.8345952616726249E-4</v>
       </c>
       <c r="L61" t="s">
@@ -2807,7 +2808,7 @@
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B62">
@@ -2831,14 +2832,14 @@
       <c r="H62" s="1">
         <v>10</v>
       </c>
-      <c r="I62" s="5">
-        <f>G62/H62</f>
+      <c r="I62" s="4">
+        <f t="shared" si="1"/>
         <v>588.29999999999995</v>
       </c>
-      <c r="J62" s="4">
+      <c r="J62" s="3">
         <v>0</v>
       </c>
-      <c r="K62" s="2">
+      <c r="K62" s="5">
         <v>0</v>
       </c>
       <c r="L62" t="s">
@@ -2846,7 +2847,7 @@
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B63">
@@ -2870,14 +2871,14 @@
       <c r="H63" s="1">
         <v>22</v>
       </c>
-      <c r="I63" s="5">
-        <f>G63/H63</f>
+      <c r="I63" s="4">
+        <f t="shared" si="1"/>
         <v>1812.6363636363637</v>
       </c>
-      <c r="J63" s="4">
+      <c r="J63" s="3">
         <v>0</v>
       </c>
-      <c r="K63" s="2">
+      <c r="K63" s="5">
         <v>0</v>
       </c>
       <c r="L63" t="s">
@@ -2885,7 +2886,7 @@
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B64">
@@ -2909,14 +2910,14 @@
       <c r="H64" s="1">
         <v>34</v>
       </c>
-      <c r="I64" s="5">
-        <f>G64/H64</f>
+      <c r="I64" s="4">
+        <f t="shared" si="1"/>
         <v>3120.9117647058824</v>
       </c>
-      <c r="J64" s="4">
+      <c r="J64" s="3">
         <v>0</v>
       </c>
-      <c r="K64" s="2">
+      <c r="K64" s="5">
         <v>0</v>
       </c>
       <c r="L64" t="s">
@@ -2924,7 +2925,7 @@
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B65">
@@ -2948,14 +2949,14 @@
       <c r="H65" s="1">
         <v>49</v>
       </c>
-      <c r="I65" s="5">
-        <f>G65/H65</f>
+      <c r="I65" s="4">
+        <f t="shared" si="1"/>
         <v>4645.4489795918371</v>
       </c>
-      <c r="J65" s="4">
+      <c r="J65" s="3">
         <v>1.1574074032516535E-8</v>
       </c>
-      <c r="K65" s="2">
+      <c r="K65" s="5">
         <v>2.0408163192029156E-2</v>
       </c>
       <c r="L65" t="s">
@@ -2963,7 +2964,7 @@
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B66">
@@ -2987,14 +2988,14 @@
       <c r="H66" s="1">
         <v>50</v>
       </c>
-      <c r="I66" s="5">
-        <f>G66/H66</f>
+      <c r="I66" s="4">
+        <f t="shared" ref="I66:I97" si="2">G66/H66</f>
         <v>5560.78</v>
       </c>
-      <c r="J66" s="4">
+      <c r="J66" s="3">
         <v>1.1574074143538837E-8</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K66" s="5">
         <v>2.0000000120035111E-2</v>
       </c>
       <c r="L66" t="s">
@@ -3002,7 +3003,7 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B67">
@@ -3026,14 +3027,14 @@
       <c r="H67" s="1">
         <v>60</v>
       </c>
-      <c r="I67" s="5">
-        <f>G67/H67</f>
+      <c r="I67" s="4">
+        <f t="shared" si="2"/>
         <v>6471.1166666666668</v>
       </c>
-      <c r="J67" s="4">
+      <c r="J67" s="3">
         <v>2.3148148176055372E-8</v>
       </c>
-      <c r="K67" s="2">
+      <c r="K67" s="5">
         <v>3.3333333373519736E-2</v>
       </c>
       <c r="L67" t="s">
@@ -3041,7 +3042,7 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B68">
@@ -3065,14 +3066,14 @@
       <c r="H68" s="1">
         <v>70</v>
       </c>
-      <c r="I68" s="5">
-        <f>G68/H68</f>
+      <c r="I68" s="4">
+        <f t="shared" si="2"/>
         <v>7641.4142857142861</v>
       </c>
-      <c r="J68" s="4">
+      <c r="J68" s="3">
         <v>2.3148148176055372E-8</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68" s="5">
         <v>2.8571428605874059E-2</v>
       </c>
       <c r="L68" t="s">
@@ -3080,7 +3081,7 @@
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B69">
@@ -3104,14 +3105,14 @@
       <c r="H69" s="1">
         <v>121</v>
       </c>
-      <c r="I69" s="5">
-        <f>G69/H69</f>
+      <c r="I69" s="4">
+        <f t="shared" si="2"/>
         <v>8231.6694214876024</v>
       </c>
-      <c r="J69" s="4">
+      <c r="J69" s="3">
         <v>5.7870370384627279E-8</v>
       </c>
-      <c r="K69" s="2">
+      <c r="K69" s="5">
         <v>4.1322314059766919E-2</v>
       </c>
       <c r="L69" t="s">
@@ -3119,7 +3120,7 @@
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B70">
@@ -3143,14 +3144,14 @@
       <c r="H70" s="1">
         <v>2384</v>
       </c>
-      <c r="I70" s="5">
-        <f>G70/H70</f>
+      <c r="I70" s="4">
+        <f t="shared" si="2"/>
         <v>6326.7361577181209</v>
       </c>
-      <c r="J70" s="4">
+      <c r="J70" s="3">
         <v>9.1435185189947532E-7</v>
       </c>
-      <c r="K70" s="2">
+      <c r="K70" s="5">
         <v>3.3137583894343403E-2</v>
       </c>
       <c r="L70" t="s">
@@ -3158,7 +3159,7 @@
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B71">
@@ -3182,14 +3183,14 @@
       <c r="H71" s="1">
         <v>753</v>
       </c>
-      <c r="I71" s="5">
-        <f>G71/H71</f>
+      <c r="I71" s="4">
+        <f t="shared" si="2"/>
         <v>22758.896414342631</v>
       </c>
-      <c r="J71" s="4">
+      <c r="J71" s="3">
         <v>7.1759259262504926E-7</v>
       </c>
-      <c r="K71" s="2">
+      <c r="K71" s="5">
         <v>8.2337317400802468E-2</v>
       </c>
       <c r="L71" t="s">
@@ -3197,7 +3198,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B72">
@@ -3221,14 +3222,14 @@
       <c r="H72" s="1">
         <v>453</v>
       </c>
-      <c r="I72" s="5">
-        <f>G72/H72</f>
+      <c r="I72" s="4">
+        <f t="shared" si="2"/>
         <v>2487.0397350993376</v>
       </c>
-      <c r="J72" s="4">
+      <c r="J72" s="3">
         <v>3.4722222319594209E-8</v>
       </c>
-      <c r="K72" s="2">
+      <c r="K72" s="5">
         <v>6.6225165748630011E-3</v>
       </c>
       <c r="L72" t="s">
@@ -3236,7 +3237,7 @@
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B73">
@@ -3260,14 +3261,14 @@
       <c r="H73" s="1">
         <v>12956</v>
       </c>
-      <c r="I73" s="5">
-        <f>G73/H73</f>
+      <c r="I73" s="4">
+        <f t="shared" si="2"/>
         <v>5645.0003859215803</v>
       </c>
-      <c r="J73" s="4">
+      <c r="J73" s="3">
         <v>1.8981481481050722E-6</v>
       </c>
-      <c r="K73" s="2">
+      <c r="K73" s="5">
         <v>1.2658227847814004E-2</v>
       </c>
       <c r="L73" t="s">
@@ -3275,7 +3276,7 @@
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B74">
@@ -3299,14 +3300,14 @@
       <c r="H74" s="1">
         <v>36423</v>
       </c>
-      <c r="I74" s="5">
-        <f>G74/H74</f>
+      <c r="I74" s="4">
+        <f t="shared" si="2"/>
         <v>8895.0003569173332</v>
       </c>
-      <c r="J74" s="4">
+      <c r="J74" s="3">
         <v>8.6921296295061623E-6</v>
       </c>
-      <c r="K74" s="2">
+      <c r="K74" s="5">
         <v>2.0618839743824849E-2</v>
       </c>
       <c r="L74" t="s">
@@ -3314,7 +3315,7 @@
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B75">
@@ -3338,14 +3339,14 @@
       <c r="H75" s="1">
         <v>8354</v>
       </c>
-      <c r="I75" s="5">
-        <f>G75/H75</f>
+      <c r="I75" s="4">
+        <f t="shared" si="2"/>
         <v>11593.002274359587</v>
       </c>
-      <c r="J75" s="4">
+      <c r="J75" s="3">
         <v>2.2800925926214077E-6</v>
       </c>
-      <c r="K75" s="2">
+      <c r="K75" s="5">
         <v>2.3581517836065314E-2</v>
       </c>
       <c r="L75" t="s">
@@ -3353,7 +3354,7 @@
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B76">
@@ -3377,14 +3378,14 @@
       <c r="H76" s="1">
         <v>93512</v>
       </c>
-      <c r="I76" s="5">
-        <f>G76/H76</f>
+      <c r="I76" s="4">
+        <f t="shared" si="2"/>
         <v>15395.00016040722</v>
       </c>
-      <c r="J76" s="4">
+      <c r="J76" s="3">
         <v>3.1412037036937512E-5</v>
       </c>
-      <c r="K76" s="2">
+      <c r="K76" s="5">
         <v>2.9023013089137236E-2</v>
       </c>
       <c r="L76" t="s">
@@ -3392,7 +3393,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B77">
@@ -3416,14 +3417,14 @@
       <c r="H77" s="1">
         <v>24905</v>
       </c>
-      <c r="I77" s="5">
-        <f>G77/H77</f>
+      <c r="I77" s="4">
+        <f t="shared" si="2"/>
         <v>18369.000361373219</v>
       </c>
-      <c r="J77" s="4">
+      <c r="J77" s="3">
         <v>9.7569444443834641E-6</v>
       </c>
-      <c r="K77" s="2">
+      <c r="K77" s="5">
         <v>3.3848624773930185E-2</v>
       </c>
       <c r="L77" t="s">
@@ -3431,7 +3432,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B78">
@@ -3455,14 +3456,14 @@
       <c r="H78" s="1">
         <v>18457</v>
       </c>
-      <c r="I78" s="5">
-        <f>G78/H78</f>
+      <c r="I78" s="4">
+        <f t="shared" si="2"/>
         <v>21527.000270899931</v>
       </c>
-      <c r="J78" s="4">
+      <c r="J78" s="3">
         <v>9.2939814814174682E-6</v>
       </c>
-      <c r="K78" s="2">
+      <c r="K78" s="5">
         <v>4.3506528688002886E-2</v>
       </c>
       <c r="L78" t="s">
@@ -3470,7 +3471,7 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B79">
@@ -3494,14 +3495,14 @@
       <c r="H79" s="1">
         <v>3159489</v>
       </c>
-      <c r="I79" s="5">
-        <f>G79/H79</f>
+      <c r="I79" s="4">
+        <f t="shared" si="2"/>
         <v>24685.000001266028</v>
       </c>
-      <c r="J79" s="4">
+      <c r="J79" s="3">
         <v>1.9458449074074569E-3</v>
       </c>
-      <c r="K79" s="2">
+      <c r="K79" s="5">
         <v>5.3211452864689285E-2</v>
       </c>
       <c r="L79" t="s">
@@ -3509,7 +3510,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B80">
@@ -3533,14 +3534,14 @@
       <c r="H80" s="1">
         <v>830596</v>
       </c>
-      <c r="I80" s="5">
-        <f>G80/H80</f>
+      <c r="I80" s="4">
+        <f t="shared" si="2"/>
         <v>27935.000020467232</v>
       </c>
-      <c r="J80" s="4">
+      <c r="J80" s="3">
         <v>6.2414351851858285E-4</v>
       </c>
-      <c r="K80" s="2">
+      <c r="K80" s="5">
         <v>6.4924463878956271E-2</v>
       </c>
       <c r="L80" t="s">
@@ -3548,7 +3549,7 @@
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B81">
@@ -3572,14 +3573,14 @@
       <c r="H81" s="1">
         <v>98964209</v>
       </c>
-      <c r="I81" s="5">
-        <f>G81/H81</f>
+      <c r="I81" s="4">
+        <f t="shared" si="2"/>
         <v>30725.000000171778</v>
       </c>
-      <c r="J81" s="4">
+      <c r="J81" s="3">
         <v>6.9182546296296249E-2</v>
       </c>
-      <c r="K81" s="2">
+      <c r="K81" s="5">
         <v>6.0399330832826593E-2</v>
       </c>
       <c r="L81" t="s">
@@ -3593,5 +3594,6 @@
     <sortCondition ref="B2:B81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>